<commit_message>
Add more cases for get xls with missing values
</commit_message>
<xml_diff>
--- a/tests/get_with_missing_values_xlsx/input.xlsx
+++ b/tests/get_with_missing_values_xlsx/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CREAF\dev\models\excel_bugs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CREAF\dev\pysd\tests\test-models\tests\get_with_missing_values_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8EDC5-B5C0-4CDD-AE17-4388A2FDF85E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6ECB56-0FE6-4611-85DC-748610385CA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="14400" windowHeight="7335" xr2:uid="{87F1062C-A5F2-41EA-A497-5D2D6861176B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{87F1062C-A5F2-41EA-A497-5D2D6861176B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,8 +71,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5FCF98D-7B06-497C-BE77-766F253DE855}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,9 +433,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>5</v>
-      </c>
+      <c r="B5" s="2"/>
       <c r="D5">
         <v>2</v>
       </c>
@@ -443,6 +451,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="C6">
         <v>3</v>
       </c>
@@ -469,6 +478,7 @@
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8" s="2"/>
       <c r="D8">
         <v>4</v>
       </c>
@@ -548,5 +558,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>